<commit_message>
agrego en formato osd
</commit_message>
<xml_diff>
--- a/GIT_COMANDOS.xlsx
+++ b/GIT_COMANDOS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18f14d8a0bb87c38/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18f14d8a0bb87c38/Desktop/GIT RESUMEN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{D6C8211A-8708-4916-A791-10AFC4FEBADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF858B9A-955D-4AEA-98C4-CF935DE9E7DB}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{D6C8211A-8708-4916-A791-10AFC4FEBADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC8E3046-26E8-4BA9-96FC-4933068F79B3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A15D5325-8E5E-4DBD-9291-1C7C0198287E}"/>
   </bookViews>
@@ -593,14 +593,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -619,6 +613,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,11 +946,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -959,7 +959,7 @@
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -970,552 +970,552 @@
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="16"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="17"/>
     </row>
     <row r="5" spans="1:3" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="15"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="15"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="15"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="15"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="15"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="17"/>
+      <c r="C21" s="15"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="15"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="15"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="15"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="17"/>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="17"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="17"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="17"/>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="17"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="17"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="17"/>
+      <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="17"/>
+      <c r="C37" s="15"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="17"/>
+      <c r="C38" s="15"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="17"/>
+      <c r="C39" s="15"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="17"/>
+      <c r="C40" s="15"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="17"/>
+      <c r="C41" s="15"/>
     </row>
     <row r="42" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="17"/>
+      <c r="C42" s="15"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="17"/>
+      <c r="C43" s="15"/>
     </row>
     <row r="44" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="17"/>
+      <c r="C44" s="15"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="17"/>
+      <c r="C45" s="15"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="17"/>
+      <c r="C46" s="15"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="17"/>
+      <c r="C47" s="15"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="17"/>
+      <c r="C48" s="15"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C49" s="17"/>
+      <c r="C49" s="15"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="17"/>
+      <c r="C50" s="15"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="17"/>
+      <c r="C51" s="15"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="17"/>
+      <c r="C52" s="15"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="17"/>
+      <c r="C53" s="15"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="17"/>
+      <c r="C54" s="15"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C55" s="17"/>
+      <c r="C55" s="15"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C56" s="17"/>
+      <c r="C56" s="15"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C57" s="17"/>
+      <c r="C57" s="15"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="17"/>
+      <c r="C58" s="15"/>
     </row>
     <row r="59" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="C59" s="17"/>
+      <c r="C59" s="15"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="17"/>
+      <c r="C60" s="15"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="17"/>
+      <c r="C61" s="15"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C62" s="17"/>
+      <c r="C62" s="15"/>
     </row>
     <row r="63" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="15" t="s">
+      <c r="A63" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C63" s="17"/>
+      <c r="C63" s="15"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
+      <c r="A64" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C64" s="17"/>
+      <c r="C64" s="15"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>

</xml_diff>